<commit_message>
nmv 15 12 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 7.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 7.2 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC19BF1-1AD4-497A-9FE7-B0FE779817EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB872E44-0985-47C7-AFE1-037EFC459106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6068" uniqueCount="1180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6071" uniqueCount="1181">
   <si>
     <t>Passage</t>
   </si>
@@ -3552,9 +3552,6 @@
     <t>anvanu</t>
   </si>
   <si>
-    <t>NE+NRE</t>
-  </si>
-  <si>
     <t>LE</t>
   </si>
   <si>
@@ -3568,6 +3565,12 @@
   </si>
   <si>
     <t>anu cChandaH</t>
+  </si>
+  <si>
+    <t>prA~g. yAnti (swara bakthi??)</t>
+  </si>
+  <si>
+    <t>P[s]</t>
   </si>
 </sst>
 </file>
@@ -3723,7 +3726,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3751,6 +3754,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3782,7 +3791,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3968,6 +3977,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3983,7 +3995,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4266,12 +4281,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V2728"/>
+  <dimension ref="A1:V2331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2315" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N2331" sqref="N2331"/>
+      <selection pane="bottomLeft" activeCell="S2331" sqref="S2331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -10274,7 +10289,7 @@
         <f t="shared" si="8"/>
         <v>146</v>
       </c>
-      <c r="N147" s="46" t="s">
+      <c r="N147" s="70" t="s">
         <v>212</v>
       </c>
       <c r="O147" s="7"/>
@@ -10287,7 +10302,11 @@
       <c r="V147" s="46"/>
     </row>
     <row r="148" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A148" s="62"/>
+      <c r="A148" s="57" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B148" s="57"/>
+      <c r="C148" s="57"/>
       <c r="D148" s="24"/>
       <c r="H148" s="53" t="s">
         <v>79</v>
@@ -10310,7 +10329,7 @@
         <f t="shared" si="8"/>
         <v>147</v>
       </c>
-      <c r="N148" s="46" t="s">
+      <c r="N148" s="70" t="s">
         <v>213</v>
       </c>
       <c r="O148" s="7"/>
@@ -22468,7 +22487,7 @@
       <c r="S499" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="T499" s="8" t="s">
+      <c r="T499" s="69" t="s">
         <v>78</v>
       </c>
       <c r="U499" s="8"/>
@@ -22505,8 +22524,12 @@
       <c r="P500" s="8"/>
       <c r="Q500" s="8"/>
       <c r="R500" s="8"/>
-      <c r="S500" s="8"/>
-      <c r="T500" s="8"/>
+      <c r="S500" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="T500" s="69" t="s">
+        <v>1180</v>
+      </c>
       <c r="U500" s="8"/>
       <c r="V500" s="46"/>
     </row>
@@ -27593,7 +27616,7 @@
         <v>61</v>
       </c>
       <c r="N648" s="47" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="O648" s="8" t="s">
         <v>70</v>
@@ -41264,36 +41287,36 @@
       </c>
     </row>
     <row r="1068" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I1068" s="63" t="s">
+      <c r="I1068" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="J1068" s="64">
+      <c r="J1068" s="52">
         <v>23</v>
       </c>
-      <c r="K1068" s="65">
+      <c r="K1068" s="6">
         <f t="shared" si="48"/>
         <v>1067</v>
       </c>
-      <c r="L1068" s="65">
+      <c r="L1068" s="6">
         <v>1</v>
       </c>
-      <c r="M1068" s="65">
+      <c r="M1068" s="6">
         <f t="shared" si="50"/>
         <v>51</v>
       </c>
-      <c r="N1068" s="66" t="s">
+      <c r="N1068" s="46" t="s">
         <v>1053</v>
       </c>
-      <c r="O1068" s="67" t="s">
+      <c r="O1068" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="P1068" s="67"/>
-      <c r="Q1068" s="67"/>
-      <c r="R1068" s="67"/>
-      <c r="S1068" s="67"/>
-      <c r="T1068" s="67"/>
-      <c r="U1068" s="67"/>
-      <c r="V1068" s="66" t="s">
+      <c r="P1068" s="8"/>
+      <c r="Q1068" s="8"/>
+      <c r="R1068" s="8"/>
+      <c r="S1068" s="8"/>
+      <c r="T1068" s="8"/>
+      <c r="U1068" s="8"/>
+      <c r="V1068" s="46" t="s">
         <v>546</v>
       </c>
     </row>
@@ -42476,7 +42499,6 @@
       <c r="P1104" s="8"/>
       <c r="Q1104" s="8"/>
       <c r="R1104" s="8"/>
-      <c r="S1104" s="8"/>
       <c r="T1104" s="8"/>
       <c r="U1104" s="8"/>
       <c r="V1104" s="46"/>
@@ -42508,8 +42530,12 @@
       <c r="P1105" s="8"/>
       <c r="Q1105" s="8"/>
       <c r="R1105" s="8"/>
-      <c r="S1105" s="8"/>
-      <c r="T1105" s="8"/>
+      <c r="S1105" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="T1105" s="8" t="s">
+        <v>102</v>
+      </c>
       <c r="U1105" s="8"/>
       <c r="V1105" s="46"/>
     </row>
@@ -42902,7 +42928,7 @@
         <f t="shared" si="53"/>
         <v>100</v>
       </c>
-      <c r="N1117" s="66" t="s">
+      <c r="N1117" s="46" t="s">
         <v>572</v>
       </c>
       <c r="O1117" s="7"/>
@@ -44491,35 +44517,35 @@
     </row>
     <row r="1167" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H1167" s="31"/>
-      <c r="I1167" s="49" t="s">
+      <c r="I1167" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="J1167" s="52">
+      <c r="J1167" s="65">
         <v>24</v>
       </c>
-      <c r="K1167" s="6">
+      <c r="K1167" s="66">
         <f t="shared" si="54"/>
         <v>1166</v>
       </c>
-      <c r="L1167" s="6">
+      <c r="L1167" s="66">
         <f t="shared" si="55"/>
         <v>50</v>
       </c>
-      <c r="M1167" s="6">
+      <c r="M1167" s="66">
         <f t="shared" si="56"/>
         <v>150</v>
       </c>
-      <c r="N1167" s="46" t="s">
+      <c r="N1167" s="67" t="s">
         <v>590</v>
       </c>
-      <c r="O1167" s="8"/>
-      <c r="P1167" s="8"/>
-      <c r="Q1167" s="8"/>
-      <c r="R1167" s="8"/>
-      <c r="S1167" s="8"/>
-      <c r="T1167" s="8"/>
-      <c r="U1167" s="8"/>
-      <c r="V1167" s="46"/>
+      <c r="O1167" s="68"/>
+      <c r="P1167" s="68"/>
+      <c r="Q1167" s="68"/>
+      <c r="R1167" s="68"/>
+      <c r="S1167" s="68"/>
+      <c r="T1167" s="68"/>
+      <c r="U1167" s="68"/>
+      <c r="V1167" s="67"/>
     </row>
     <row r="1168" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1168" s="49" t="s">
@@ -51396,7 +51422,7 @@
     </row>
     <row r="1381" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1381" s="62" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C1381" s="41"/>
       <c r="H1381" s="34"/>
@@ -51418,7 +51444,7 @@
         <f t="shared" si="65"/>
         <v>89</v>
       </c>
-      <c r="N1381" s="68" t="s">
+      <c r="N1381" s="63" t="s">
         <v>658</v>
       </c>
       <c r="O1381" s="7"/>
@@ -51454,7 +51480,7 @@
         <f t="shared" si="65"/>
         <v>90</v>
       </c>
-      <c r="N1382" s="68" t="s">
+      <c r="N1382" s="63" t="s">
         <v>984</v>
       </c>
       <c r="O1382" s="8" t="s">
@@ -53872,7 +53898,7 @@
     </row>
     <row r="1456" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1456" s="62" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C1456" s="41"/>
       <c r="I1456" s="49" t="s">
@@ -53928,7 +53954,7 @@
         <f t="shared" si="68"/>
         <v>165</v>
       </c>
-      <c r="N1457" s="68" t="s">
+      <c r="N1457" s="63" t="s">
         <v>658</v>
       </c>
       <c r="O1457" s="7"/>
@@ -53965,7 +53991,7 @@
         <f t="shared" si="68"/>
         <v>166</v>
       </c>
-      <c r="N1458" s="68" t="s">
+      <c r="N1458" s="63" t="s">
         <v>984</v>
       </c>
       <c r="O1458" s="8" t="s">
@@ -53976,9 +54002,7 @@
       <c r="R1458" s="8"/>
       <c r="S1458" s="8"/>
       <c r="T1458" s="8"/>
-      <c r="U1458" s="8" t="s">
-        <v>1174</v>
-      </c>
+      <c r="U1458" s="8"/>
       <c r="V1458" s="46"/>
     </row>
     <row r="1459" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -55908,7 +55932,7 @@
     </row>
     <row r="1517" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1517" s="62" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C1517" s="41"/>
       <c r="I1517" s="49" t="s">
@@ -55929,7 +55953,7 @@
         <f t="shared" si="71"/>
         <v>225</v>
       </c>
-      <c r="N1517" s="68" t="s">
+      <c r="N1517" s="63" t="s">
         <v>658</v>
       </c>
       <c r="O1517" s="7"/>
@@ -55964,7 +55988,7 @@
         <f t="shared" si="71"/>
         <v>226</v>
       </c>
-      <c r="N1518" s="68" t="s">
+      <c r="N1518" s="63" t="s">
         <v>984</v>
       </c>
       <c r="O1518" s="8" t="s">
@@ -55975,9 +55999,7 @@
       <c r="R1518" s="8"/>
       <c r="S1518" s="8"/>
       <c r="T1518" s="8"/>
-      <c r="U1518" s="8" t="s">
-        <v>1174</v>
-      </c>
+      <c r="U1518" s="69"/>
       <c r="V1518" s="46"/>
     </row>
     <row r="1519" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
@@ -62185,7 +62207,7 @@
         <f t="shared" si="83"/>
         <v>100</v>
       </c>
-      <c r="N1743" s="66" t="s">
+      <c r="N1743" s="46" t="s">
         <v>135</v>
       </c>
       <c r="V1743" s="46"/>
@@ -66756,10 +66778,10 @@
         <v>809</v>
       </c>
       <c r="S1922" s="1" t="s">
+        <v>1174</v>
+      </c>
+      <c r="T1922" s="1" t="s">
         <v>1175</v>
-      </c>
-      <c r="T1922" s="1" t="s">
-        <v>1176</v>
       </c>
       <c r="V1922" s="46"/>
     </row>
@@ -77128,1991 +77150,6 @@
       <c r="V2331" s="46" t="s">
         <v>1158</v>
       </c>
-    </row>
-    <row r="2332" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2332" s="49"/>
-      <c r="N2332" s="46"/>
-      <c r="V2332" s="46"/>
-    </row>
-    <row r="2333" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2333" s="49"/>
-      <c r="N2333" s="46"/>
-      <c r="V2333" s="46"/>
-    </row>
-    <row r="2334" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2334" s="49"/>
-      <c r="N2334" s="46"/>
-      <c r="V2334" s="46"/>
-    </row>
-    <row r="2335" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2335" s="49"/>
-      <c r="N2335" s="46"/>
-      <c r="V2335" s="46"/>
-    </row>
-    <row r="2336" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2336" s="49"/>
-      <c r="N2336" s="46"/>
-      <c r="V2336" s="46"/>
-    </row>
-    <row r="2337" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2337" s="49"/>
-      <c r="N2337" s="46"/>
-      <c r="V2337" s="46"/>
-    </row>
-    <row r="2338" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2338" s="49"/>
-      <c r="N2338" s="46"/>
-      <c r="V2338" s="46"/>
-    </row>
-    <row r="2339" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2339" s="49"/>
-      <c r="N2339" s="46"/>
-      <c r="V2339" s="46"/>
-    </row>
-    <row r="2340" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2340" s="49"/>
-      <c r="N2340" s="46"/>
-      <c r="V2340" s="46"/>
-    </row>
-    <row r="2341" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2341" s="49"/>
-      <c r="N2341" s="46"/>
-      <c r="V2341" s="46"/>
-    </row>
-    <row r="2342" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2342" s="49"/>
-      <c r="N2342" s="46"/>
-      <c r="V2342" s="46"/>
-    </row>
-    <row r="2343" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2343" s="49"/>
-      <c r="N2343" s="46"/>
-      <c r="V2343" s="46"/>
-    </row>
-    <row r="2344" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2344" s="49"/>
-      <c r="N2344" s="46"/>
-      <c r="V2344" s="46"/>
-    </row>
-    <row r="2345" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2345" s="49"/>
-      <c r="N2345" s="46"/>
-      <c r="V2345" s="46"/>
-    </row>
-    <row r="2346" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2346" s="49"/>
-      <c r="N2346" s="46"/>
-      <c r="V2346" s="46"/>
-    </row>
-    <row r="2347" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2347" s="49"/>
-      <c r="N2347" s="46"/>
-      <c r="V2347" s="46"/>
-    </row>
-    <row r="2348" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2348" s="49"/>
-      <c r="N2348" s="46"/>
-      <c r="V2348" s="46"/>
-    </row>
-    <row r="2349" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2349" s="49"/>
-      <c r="N2349" s="46"/>
-      <c r="V2349" s="46"/>
-    </row>
-    <row r="2350" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2350" s="49"/>
-      <c r="N2350" s="46"/>
-      <c r="V2350" s="46"/>
-    </row>
-    <row r="2351" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2351" s="49"/>
-      <c r="N2351" s="46"/>
-      <c r="V2351" s="46"/>
-    </row>
-    <row r="2352" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2352" s="49"/>
-      <c r="N2352" s="46"/>
-      <c r="V2352" s="46"/>
-    </row>
-    <row r="2353" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2353" s="49"/>
-      <c r="N2353" s="46"/>
-      <c r="V2353" s="46"/>
-    </row>
-    <row r="2354" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2354" s="49"/>
-      <c r="N2354" s="46"/>
-      <c r="V2354" s="46"/>
-    </row>
-    <row r="2355" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2355" s="49"/>
-      <c r="N2355" s="46"/>
-      <c r="V2355" s="46"/>
-    </row>
-    <row r="2356" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2356" s="49"/>
-      <c r="N2356" s="46"/>
-      <c r="V2356" s="46"/>
-    </row>
-    <row r="2357" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2357" s="49"/>
-      <c r="N2357" s="46"/>
-      <c r="V2357" s="46"/>
-    </row>
-    <row r="2358" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2358" s="49"/>
-      <c r="N2358" s="46"/>
-      <c r="V2358" s="46"/>
-    </row>
-    <row r="2359" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2359" s="49"/>
-      <c r="N2359" s="46"/>
-      <c r="V2359" s="46"/>
-    </row>
-    <row r="2360" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2360" s="49"/>
-      <c r="N2360" s="46"/>
-      <c r="V2360" s="46"/>
-    </row>
-    <row r="2361" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2361" s="49"/>
-      <c r="N2361" s="46"/>
-      <c r="V2361" s="46"/>
-    </row>
-    <row r="2362" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2362" s="49"/>
-      <c r="N2362" s="46"/>
-      <c r="V2362" s="46"/>
-    </row>
-    <row r="2363" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2363" s="49"/>
-      <c r="N2363" s="46"/>
-      <c r="V2363" s="46"/>
-    </row>
-    <row r="2364" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2364" s="49"/>
-      <c r="N2364" s="46"/>
-      <c r="V2364" s="46"/>
-    </row>
-    <row r="2365" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2365" s="49"/>
-      <c r="N2365" s="46"/>
-      <c r="V2365" s="46"/>
-    </row>
-    <row r="2366" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2366" s="49"/>
-      <c r="N2366" s="46"/>
-      <c r="V2366" s="46"/>
-    </row>
-    <row r="2367" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2367" s="49"/>
-      <c r="N2367" s="46"/>
-      <c r="V2367" s="46"/>
-    </row>
-    <row r="2368" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2368" s="49"/>
-      <c r="N2368" s="46"/>
-      <c r="V2368" s="46"/>
-    </row>
-    <row r="2369" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2369" s="49"/>
-      <c r="N2369" s="46"/>
-      <c r="V2369" s="46"/>
-    </row>
-    <row r="2370" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2370" s="49"/>
-      <c r="N2370" s="46"/>
-      <c r="V2370" s="46"/>
-    </row>
-    <row r="2371" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2371" s="49"/>
-      <c r="N2371" s="46"/>
-      <c r="V2371" s="46"/>
-    </row>
-    <row r="2372" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2372" s="49"/>
-      <c r="N2372" s="46"/>
-      <c r="V2372" s="46"/>
-    </row>
-    <row r="2373" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2373" s="49"/>
-      <c r="N2373" s="46"/>
-      <c r="V2373" s="46"/>
-    </row>
-    <row r="2374" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2374" s="49"/>
-      <c r="N2374" s="46"/>
-      <c r="V2374" s="46"/>
-    </row>
-    <row r="2375" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2375" s="49"/>
-      <c r="N2375" s="46"/>
-      <c r="V2375" s="46"/>
-    </row>
-    <row r="2376" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2376" s="49"/>
-      <c r="N2376" s="46"/>
-      <c r="V2376" s="46"/>
-    </row>
-    <row r="2377" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2377" s="49"/>
-      <c r="N2377" s="46"/>
-      <c r="V2377" s="46"/>
-    </row>
-    <row r="2378" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2378" s="49"/>
-      <c r="N2378" s="46"/>
-      <c r="V2378" s="46"/>
-    </row>
-    <row r="2379" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2379" s="49"/>
-      <c r="N2379" s="46"/>
-      <c r="V2379" s="46"/>
-    </row>
-    <row r="2380" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2380" s="49"/>
-      <c r="N2380" s="46"/>
-      <c r="V2380" s="46"/>
-    </row>
-    <row r="2381" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2381" s="49"/>
-      <c r="N2381" s="46"/>
-      <c r="V2381" s="46"/>
-    </row>
-    <row r="2382" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2382" s="49"/>
-      <c r="N2382" s="46"/>
-      <c r="V2382" s="46"/>
-    </row>
-    <row r="2383" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2383" s="49"/>
-      <c r="N2383" s="46"/>
-      <c r="V2383" s="46"/>
-    </row>
-    <row r="2384" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2384" s="49"/>
-      <c r="N2384" s="46"/>
-      <c r="V2384" s="46"/>
-    </row>
-    <row r="2385" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2385" s="49"/>
-      <c r="N2385" s="46"/>
-      <c r="V2385" s="46"/>
-    </row>
-    <row r="2386" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2386" s="49"/>
-      <c r="N2386" s="46"/>
-      <c r="V2386" s="46"/>
-    </row>
-    <row r="2387" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2387" s="49"/>
-      <c r="N2387" s="46"/>
-      <c r="V2387" s="46"/>
-    </row>
-    <row r="2388" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2388" s="49"/>
-      <c r="N2388" s="46"/>
-      <c r="V2388" s="46"/>
-    </row>
-    <row r="2389" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2389" s="49"/>
-      <c r="N2389" s="46"/>
-      <c r="V2389" s="46"/>
-    </row>
-    <row r="2390" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2390" s="49"/>
-      <c r="N2390" s="46"/>
-      <c r="V2390" s="46"/>
-    </row>
-    <row r="2391" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2391" s="49"/>
-      <c r="N2391" s="46"/>
-      <c r="V2391" s="46"/>
-    </row>
-    <row r="2392" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2392" s="49"/>
-      <c r="N2392" s="46"/>
-      <c r="V2392" s="46"/>
-    </row>
-    <row r="2393" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2393" s="49"/>
-      <c r="N2393" s="46"/>
-      <c r="V2393" s="46"/>
-    </row>
-    <row r="2394" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2394" s="49"/>
-      <c r="N2394" s="46"/>
-      <c r="V2394" s="46"/>
-    </row>
-    <row r="2395" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2395" s="49"/>
-      <c r="N2395" s="46"/>
-      <c r="V2395" s="46"/>
-    </row>
-    <row r="2396" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2396" s="49"/>
-      <c r="N2396" s="46"/>
-      <c r="V2396" s="46"/>
-    </row>
-    <row r="2397" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2397" s="49"/>
-      <c r="N2397" s="46"/>
-      <c r="V2397" s="46"/>
-    </row>
-    <row r="2398" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2398" s="49"/>
-      <c r="N2398" s="46"/>
-      <c r="V2398" s="46"/>
-    </row>
-    <row r="2399" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2399" s="49"/>
-      <c r="N2399" s="46"/>
-      <c r="V2399" s="46"/>
-    </row>
-    <row r="2400" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2400" s="49"/>
-      <c r="N2400" s="46"/>
-      <c r="V2400" s="46"/>
-    </row>
-    <row r="2401" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2401" s="49"/>
-      <c r="N2401" s="46"/>
-      <c r="V2401" s="46"/>
-    </row>
-    <row r="2402" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2402" s="49"/>
-      <c r="N2402" s="46"/>
-      <c r="V2402" s="46"/>
-    </row>
-    <row r="2403" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2403" s="49"/>
-      <c r="N2403" s="46"/>
-      <c r="V2403" s="46"/>
-    </row>
-    <row r="2404" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2404" s="49"/>
-      <c r="N2404" s="46"/>
-      <c r="V2404" s="46"/>
-    </row>
-    <row r="2405" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2405" s="49"/>
-      <c r="N2405" s="46"/>
-      <c r="V2405" s="46"/>
-    </row>
-    <row r="2406" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2406" s="49"/>
-      <c r="N2406" s="46"/>
-      <c r="V2406" s="46"/>
-    </row>
-    <row r="2407" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2407" s="49"/>
-      <c r="N2407" s="46"/>
-      <c r="V2407" s="46"/>
-    </row>
-    <row r="2408" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2408" s="49"/>
-      <c r="N2408" s="46"/>
-      <c r="V2408" s="46"/>
-    </row>
-    <row r="2409" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2409" s="49"/>
-      <c r="N2409" s="46"/>
-      <c r="V2409" s="46"/>
-    </row>
-    <row r="2410" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2410" s="49"/>
-      <c r="N2410" s="46"/>
-      <c r="V2410" s="46"/>
-    </row>
-    <row r="2411" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2411" s="49"/>
-      <c r="N2411" s="46"/>
-      <c r="V2411" s="46"/>
-    </row>
-    <row r="2412" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2412" s="49"/>
-      <c r="N2412" s="46"/>
-      <c r="V2412" s="46"/>
-    </row>
-    <row r="2413" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2413" s="49"/>
-      <c r="N2413" s="46"/>
-      <c r="V2413" s="46"/>
-    </row>
-    <row r="2414" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2414" s="49"/>
-      <c r="N2414" s="46"/>
-      <c r="V2414" s="46"/>
-    </row>
-    <row r="2415" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2415" s="49"/>
-      <c r="N2415" s="46"/>
-      <c r="V2415" s="46"/>
-    </row>
-    <row r="2416" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2416" s="49"/>
-      <c r="N2416" s="46"/>
-      <c r="V2416" s="46"/>
-    </row>
-    <row r="2417" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2417" s="49"/>
-      <c r="N2417" s="46"/>
-      <c r="V2417" s="46"/>
-    </row>
-    <row r="2418" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2418" s="49"/>
-      <c r="N2418" s="46"/>
-      <c r="V2418" s="46"/>
-    </row>
-    <row r="2419" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2419" s="49"/>
-      <c r="N2419" s="46"/>
-      <c r="V2419" s="46"/>
-    </row>
-    <row r="2420" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2420" s="49"/>
-      <c r="N2420" s="46"/>
-      <c r="V2420" s="46"/>
-    </row>
-    <row r="2421" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2421" s="49"/>
-      <c r="N2421" s="46"/>
-      <c r="V2421" s="46"/>
-    </row>
-    <row r="2422" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2422" s="49"/>
-      <c r="N2422" s="46"/>
-      <c r="V2422" s="46"/>
-    </row>
-    <row r="2423" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2423" s="49"/>
-      <c r="N2423" s="46"/>
-      <c r="V2423" s="46"/>
-    </row>
-    <row r="2424" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2424" s="49"/>
-      <c r="N2424" s="46"/>
-      <c r="V2424" s="46"/>
-    </row>
-    <row r="2425" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2425" s="49"/>
-      <c r="N2425" s="46"/>
-      <c r="V2425" s="46"/>
-    </row>
-    <row r="2426" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2426" s="49"/>
-      <c r="N2426" s="46"/>
-      <c r="V2426" s="46"/>
-    </row>
-    <row r="2427" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2427" s="49"/>
-      <c r="N2427" s="46"/>
-      <c r="V2427" s="46"/>
-    </row>
-    <row r="2428" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2428" s="49"/>
-      <c r="N2428" s="46"/>
-      <c r="V2428" s="46"/>
-    </row>
-    <row r="2429" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2429" s="49"/>
-      <c r="N2429" s="46"/>
-      <c r="V2429" s="46"/>
-    </row>
-    <row r="2430" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2430" s="49"/>
-      <c r="N2430" s="46"/>
-      <c r="V2430" s="46"/>
-    </row>
-    <row r="2431" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2431" s="49"/>
-      <c r="N2431" s="46"/>
-      <c r="V2431" s="46"/>
-    </row>
-    <row r="2432" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2432" s="49"/>
-      <c r="N2432" s="46"/>
-      <c r="V2432" s="46"/>
-    </row>
-    <row r="2433" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2433" s="49"/>
-      <c r="N2433" s="46"/>
-      <c r="V2433" s="46"/>
-    </row>
-    <row r="2434" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2434" s="49"/>
-      <c r="N2434" s="46"/>
-      <c r="V2434" s="46"/>
-    </row>
-    <row r="2435" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2435" s="49"/>
-      <c r="N2435" s="46"/>
-      <c r="V2435" s="46"/>
-    </row>
-    <row r="2436" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2436" s="49"/>
-      <c r="N2436" s="46"/>
-      <c r="V2436" s="46"/>
-    </row>
-    <row r="2437" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2437" s="49"/>
-      <c r="N2437" s="46"/>
-      <c r="V2437" s="46"/>
-    </row>
-    <row r="2438" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2438" s="49"/>
-      <c r="N2438" s="46"/>
-      <c r="V2438" s="46"/>
-    </row>
-    <row r="2439" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2439" s="49"/>
-      <c r="N2439" s="46"/>
-      <c r="V2439" s="46"/>
-    </row>
-    <row r="2440" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2440" s="49"/>
-      <c r="N2440" s="46"/>
-      <c r="V2440" s="46"/>
-    </row>
-    <row r="2441" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2441" s="49"/>
-      <c r="N2441" s="46"/>
-      <c r="V2441" s="46"/>
-    </row>
-    <row r="2442" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2442" s="49"/>
-      <c r="N2442" s="46"/>
-      <c r="V2442" s="46"/>
-    </row>
-    <row r="2443" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2443" s="49"/>
-      <c r="N2443" s="46"/>
-      <c r="V2443" s="46"/>
-    </row>
-    <row r="2444" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2444" s="49"/>
-      <c r="N2444" s="46"/>
-      <c r="V2444" s="46"/>
-    </row>
-    <row r="2445" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2445" s="49"/>
-      <c r="N2445" s="46"/>
-      <c r="V2445" s="46"/>
-    </row>
-    <row r="2446" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2446" s="49"/>
-      <c r="N2446" s="46"/>
-      <c r="V2446" s="46"/>
-    </row>
-    <row r="2447" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2447" s="49"/>
-      <c r="N2447" s="46"/>
-      <c r="V2447" s="46"/>
-    </row>
-    <row r="2448" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2448" s="49"/>
-      <c r="N2448" s="46"/>
-      <c r="V2448" s="46"/>
-    </row>
-    <row r="2449" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2449" s="49"/>
-      <c r="N2449" s="46"/>
-      <c r="V2449" s="46"/>
-    </row>
-    <row r="2450" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2450" s="49"/>
-      <c r="N2450" s="46"/>
-      <c r="V2450" s="46"/>
-    </row>
-    <row r="2451" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2451" s="49"/>
-      <c r="N2451" s="46"/>
-      <c r="V2451" s="46"/>
-    </row>
-    <row r="2452" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2452" s="49"/>
-      <c r="N2452" s="47"/>
-      <c r="V2452" s="47"/>
-    </row>
-    <row r="2453" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2453" s="49"/>
-      <c r="N2453" s="46"/>
-      <c r="V2453" s="46"/>
-    </row>
-    <row r="2454" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2454" s="49"/>
-      <c r="N2454" s="46"/>
-      <c r="V2454" s="46"/>
-    </row>
-    <row r="2455" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2455" s="49"/>
-      <c r="N2455" s="46"/>
-      <c r="V2455" s="46"/>
-    </row>
-    <row r="2456" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2456" s="49"/>
-      <c r="N2456" s="46"/>
-      <c r="V2456" s="46"/>
-    </row>
-    <row r="2457" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2457" s="49"/>
-      <c r="N2457" s="46"/>
-      <c r="V2457" s="46"/>
-    </row>
-    <row r="2458" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2458" s="49"/>
-      <c r="N2458" s="46"/>
-      <c r="V2458" s="46"/>
-    </row>
-    <row r="2459" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2459" s="49"/>
-      <c r="N2459" s="46"/>
-      <c r="V2459" s="46"/>
-    </row>
-    <row r="2460" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2460" s="49"/>
-      <c r="N2460" s="46"/>
-      <c r="V2460" s="46"/>
-    </row>
-    <row r="2461" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2461" s="49"/>
-      <c r="N2461" s="46"/>
-      <c r="V2461" s="46"/>
-    </row>
-    <row r="2462" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2462" s="49"/>
-      <c r="N2462" s="46"/>
-      <c r="V2462" s="46"/>
-    </row>
-    <row r="2463" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2463" s="49"/>
-      <c r="N2463" s="46"/>
-      <c r="V2463" s="46"/>
-    </row>
-    <row r="2464" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2464" s="49"/>
-      <c r="N2464" s="46"/>
-      <c r="V2464" s="46"/>
-    </row>
-    <row r="2465" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2465" s="49"/>
-      <c r="N2465" s="46"/>
-      <c r="V2465" s="46"/>
-    </row>
-    <row r="2466" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2466" s="49"/>
-      <c r="N2466" s="46"/>
-      <c r="V2466" s="46"/>
-    </row>
-    <row r="2467" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2467" s="49"/>
-      <c r="N2467" s="46"/>
-      <c r="V2467" s="46"/>
-    </row>
-    <row r="2468" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2468" s="49"/>
-      <c r="N2468" s="46"/>
-      <c r="V2468" s="46"/>
-    </row>
-    <row r="2469" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2469" s="49"/>
-      <c r="N2469" s="46"/>
-      <c r="V2469" s="46"/>
-    </row>
-    <row r="2470" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2470" s="49"/>
-      <c r="N2470" s="46"/>
-      <c r="V2470" s="46"/>
-    </row>
-    <row r="2471" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2471" s="49"/>
-      <c r="N2471" s="46"/>
-      <c r="V2471" s="46"/>
-    </row>
-    <row r="2472" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2472" s="49"/>
-      <c r="N2472" s="46"/>
-      <c r="V2472" s="46"/>
-    </row>
-    <row r="2473" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2473" s="49"/>
-      <c r="N2473" s="46"/>
-      <c r="V2473" s="46"/>
-    </row>
-    <row r="2474" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2474" s="49"/>
-      <c r="N2474" s="46"/>
-      <c r="V2474" s="46"/>
-    </row>
-    <row r="2475" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2475" s="49"/>
-      <c r="N2475" s="46"/>
-      <c r="V2475" s="46"/>
-    </row>
-    <row r="2476" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2476" s="49"/>
-      <c r="N2476" s="46"/>
-      <c r="V2476" s="46"/>
-    </row>
-    <row r="2477" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2477" s="49"/>
-      <c r="N2477" s="46"/>
-      <c r="V2477" s="46"/>
-    </row>
-    <row r="2478" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2478" s="49"/>
-      <c r="N2478" s="46"/>
-      <c r="V2478" s="46"/>
-    </row>
-    <row r="2479" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2479" s="49"/>
-      <c r="N2479" s="46"/>
-      <c r="V2479" s="46"/>
-    </row>
-    <row r="2480" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2480" s="49"/>
-      <c r="N2480" s="46"/>
-      <c r="V2480" s="46"/>
-    </row>
-    <row r="2481" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2481" s="49"/>
-      <c r="N2481" s="46"/>
-      <c r="V2481" s="46"/>
-    </row>
-    <row r="2482" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2482" s="49"/>
-      <c r="N2482" s="46"/>
-      <c r="V2482" s="46"/>
-    </row>
-    <row r="2483" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2483" s="49"/>
-      <c r="N2483" s="46"/>
-      <c r="V2483" s="46"/>
-    </row>
-    <row r="2484" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2484" s="49"/>
-      <c r="N2484" s="46"/>
-      <c r="V2484" s="46"/>
-    </row>
-    <row r="2485" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2485" s="49"/>
-      <c r="N2485" s="46"/>
-      <c r="V2485" s="46"/>
-    </row>
-    <row r="2486" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2486" s="49"/>
-      <c r="N2486" s="46"/>
-      <c r="V2486" s="46"/>
-    </row>
-    <row r="2487" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2487" s="49"/>
-      <c r="N2487" s="46"/>
-      <c r="V2487" s="46"/>
-    </row>
-    <row r="2488" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2488" s="49"/>
-      <c r="N2488" s="46"/>
-      <c r="V2488" s="46"/>
-    </row>
-    <row r="2489" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2489" s="49"/>
-      <c r="N2489" s="46"/>
-      <c r="V2489" s="46"/>
-    </row>
-    <row r="2490" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2490" s="49"/>
-      <c r="N2490" s="46"/>
-      <c r="V2490" s="46"/>
-    </row>
-    <row r="2491" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2491" s="49"/>
-      <c r="N2491" s="46"/>
-      <c r="V2491" s="46"/>
-    </row>
-    <row r="2492" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2492" s="49"/>
-      <c r="N2492" s="46"/>
-      <c r="V2492" s="46"/>
-    </row>
-    <row r="2493" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2493" s="49"/>
-      <c r="N2493" s="46"/>
-      <c r="V2493" s="46"/>
-    </row>
-    <row r="2494" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2494" s="49"/>
-      <c r="N2494" s="46"/>
-      <c r="V2494" s="46"/>
-    </row>
-    <row r="2495" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2495" s="49"/>
-      <c r="N2495" s="46"/>
-      <c r="V2495" s="46"/>
-    </row>
-    <row r="2496" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2496" s="49"/>
-      <c r="N2496" s="46"/>
-      <c r="V2496" s="46"/>
-    </row>
-    <row r="2497" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2497" s="49"/>
-      <c r="N2497" s="46"/>
-      <c r="V2497" s="46"/>
-    </row>
-    <row r="2498" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2498" s="49"/>
-      <c r="N2498" s="46"/>
-      <c r="V2498" s="46"/>
-    </row>
-    <row r="2499" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2499" s="49"/>
-      <c r="N2499" s="46"/>
-      <c r="V2499" s="46"/>
-    </row>
-    <row r="2500" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2500" s="49"/>
-      <c r="N2500" s="46"/>
-      <c r="V2500" s="46"/>
-    </row>
-    <row r="2501" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2501" s="49"/>
-      <c r="N2501" s="46"/>
-      <c r="V2501" s="46"/>
-    </row>
-    <row r="2502" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2502" s="49"/>
-      <c r="N2502" s="46"/>
-      <c r="V2502" s="46"/>
-    </row>
-    <row r="2503" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2503" s="49"/>
-      <c r="N2503" s="46"/>
-      <c r="V2503" s="46"/>
-    </row>
-    <row r="2504" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2504" s="49"/>
-      <c r="N2504" s="46"/>
-      <c r="V2504" s="46"/>
-    </row>
-    <row r="2505" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2505" s="49"/>
-      <c r="N2505" s="46"/>
-      <c r="V2505" s="46"/>
-    </row>
-    <row r="2506" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2506" s="49"/>
-      <c r="N2506" s="46"/>
-      <c r="V2506" s="46"/>
-    </row>
-    <row r="2507" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2507" s="49"/>
-      <c r="N2507" s="46"/>
-      <c r="V2507" s="46"/>
-    </row>
-    <row r="2508" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2508" s="49"/>
-      <c r="N2508" s="46"/>
-      <c r="V2508" s="46"/>
-    </row>
-    <row r="2509" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2509" s="49"/>
-      <c r="N2509" s="46"/>
-      <c r="V2509" s="46"/>
-    </row>
-    <row r="2510" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2510" s="49"/>
-      <c r="N2510" s="46"/>
-      <c r="V2510" s="46"/>
-    </row>
-    <row r="2511" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2511" s="49"/>
-      <c r="N2511" s="46"/>
-      <c r="V2511" s="46"/>
-    </row>
-    <row r="2512" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2512" s="49"/>
-      <c r="N2512" s="46"/>
-      <c r="V2512" s="46"/>
-    </row>
-    <row r="2513" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2513" s="49"/>
-      <c r="N2513" s="46"/>
-      <c r="V2513" s="46"/>
-    </row>
-    <row r="2514" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2514" s="49"/>
-      <c r="N2514" s="46"/>
-      <c r="V2514" s="46"/>
-    </row>
-    <row r="2515" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2515" s="49"/>
-      <c r="N2515" s="46"/>
-      <c r="V2515" s="46"/>
-    </row>
-    <row r="2516" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2516" s="49"/>
-      <c r="N2516" s="46"/>
-      <c r="V2516" s="46"/>
-    </row>
-    <row r="2517" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2517" s="49"/>
-      <c r="N2517" s="46"/>
-      <c r="V2517" s="46"/>
-    </row>
-    <row r="2518" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2518" s="49"/>
-      <c r="N2518" s="46"/>
-      <c r="V2518" s="46"/>
-    </row>
-    <row r="2519" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2519" s="49"/>
-      <c r="N2519" s="46"/>
-      <c r="V2519" s="46"/>
-    </row>
-    <row r="2520" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2520" s="49"/>
-      <c r="N2520" s="46"/>
-      <c r="V2520" s="46"/>
-    </row>
-    <row r="2521" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2521" s="49"/>
-      <c r="N2521" s="46"/>
-      <c r="V2521" s="46"/>
-    </row>
-    <row r="2522" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2522" s="49"/>
-      <c r="N2522" s="46"/>
-      <c r="V2522" s="46"/>
-    </row>
-    <row r="2523" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2523" s="49"/>
-      <c r="N2523" s="46"/>
-      <c r="V2523" s="46"/>
-    </row>
-    <row r="2524" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2524" s="49"/>
-      <c r="N2524" s="46"/>
-      <c r="V2524" s="46"/>
-    </row>
-    <row r="2525" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2525" s="49"/>
-      <c r="N2525" s="46"/>
-      <c r="V2525" s="46"/>
-    </row>
-    <row r="2526" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2526" s="49"/>
-      <c r="N2526" s="46"/>
-      <c r="V2526" s="46"/>
-    </row>
-    <row r="2527" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2527" s="49"/>
-      <c r="N2527" s="46"/>
-      <c r="V2527" s="46"/>
-    </row>
-    <row r="2528" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2528" s="49"/>
-      <c r="N2528" s="46"/>
-      <c r="V2528" s="46"/>
-    </row>
-    <row r="2529" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2529" s="49"/>
-      <c r="N2529" s="46"/>
-      <c r="V2529" s="46"/>
-    </row>
-    <row r="2530" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2530" s="49"/>
-      <c r="N2530" s="46"/>
-      <c r="V2530" s="46"/>
-    </row>
-    <row r="2531" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2531" s="49"/>
-      <c r="N2531" s="46"/>
-      <c r="V2531" s="46"/>
-    </row>
-    <row r="2532" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2532" s="49"/>
-      <c r="N2532" s="46"/>
-      <c r="V2532" s="46"/>
-    </row>
-    <row r="2533" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2533" s="49"/>
-      <c r="N2533" s="46"/>
-      <c r="V2533" s="46"/>
-    </row>
-    <row r="2534" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2534" s="49"/>
-      <c r="N2534" s="46"/>
-      <c r="V2534" s="46"/>
-    </row>
-    <row r="2535" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2535" s="49"/>
-      <c r="N2535" s="46"/>
-      <c r="V2535" s="46"/>
-    </row>
-    <row r="2536" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2536" s="49"/>
-      <c r="N2536" s="46"/>
-      <c r="V2536" s="46"/>
-    </row>
-    <row r="2537" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2537" s="49"/>
-      <c r="N2537" s="46"/>
-      <c r="V2537" s="46"/>
-    </row>
-    <row r="2538" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2538" s="49"/>
-      <c r="N2538" s="46"/>
-      <c r="V2538" s="46"/>
-    </row>
-    <row r="2539" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2539" s="49"/>
-      <c r="N2539" s="46"/>
-      <c r="V2539" s="46"/>
-    </row>
-    <row r="2540" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2540" s="49"/>
-      <c r="N2540" s="46"/>
-      <c r="V2540" s="46"/>
-    </row>
-    <row r="2541" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2541" s="49"/>
-      <c r="N2541" s="46"/>
-      <c r="V2541" s="46"/>
-    </row>
-    <row r="2542" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2542" s="49"/>
-      <c r="N2542" s="46"/>
-      <c r="V2542" s="46"/>
-    </row>
-    <row r="2543" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2543" s="49"/>
-      <c r="N2543" s="46"/>
-      <c r="V2543" s="46"/>
-    </row>
-    <row r="2544" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2544" s="49"/>
-      <c r="N2544" s="46"/>
-      <c r="V2544" s="46"/>
-    </row>
-    <row r="2545" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2545" s="49"/>
-      <c r="N2545" s="46"/>
-      <c r="V2545" s="46"/>
-    </row>
-    <row r="2546" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2546" s="49"/>
-      <c r="N2546" s="46"/>
-      <c r="V2546" s="46"/>
-    </row>
-    <row r="2547" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2547" s="49"/>
-      <c r="N2547" s="46"/>
-      <c r="V2547" s="46"/>
-    </row>
-    <row r="2548" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2548" s="49"/>
-      <c r="N2548" s="46"/>
-      <c r="V2548" s="46"/>
-    </row>
-    <row r="2549" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2549" s="49"/>
-      <c r="N2549" s="46"/>
-      <c r="V2549" s="46"/>
-    </row>
-    <row r="2550" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2550" s="49"/>
-      <c r="N2550" s="46"/>
-      <c r="V2550" s="46"/>
-    </row>
-    <row r="2551" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2551" s="49"/>
-      <c r="N2551" s="46"/>
-      <c r="V2551" s="46"/>
-    </row>
-    <row r="2552" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2552" s="49"/>
-      <c r="N2552" s="46"/>
-      <c r="V2552" s="46"/>
-    </row>
-    <row r="2553" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2553" s="49"/>
-      <c r="N2553" s="46"/>
-      <c r="V2553" s="46"/>
-    </row>
-    <row r="2554" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2554" s="49"/>
-      <c r="N2554" s="46"/>
-      <c r="V2554" s="46"/>
-    </row>
-    <row r="2555" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2555" s="49"/>
-      <c r="N2555" s="46"/>
-      <c r="V2555" s="46"/>
-    </row>
-    <row r="2556" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2556" s="49"/>
-      <c r="N2556" s="46"/>
-      <c r="V2556" s="46"/>
-    </row>
-    <row r="2557" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2557" s="49"/>
-      <c r="N2557" s="46"/>
-      <c r="V2557" s="46"/>
-    </row>
-    <row r="2558" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2558" s="49"/>
-      <c r="N2558" s="46"/>
-      <c r="V2558" s="46"/>
-    </row>
-    <row r="2559" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2559" s="49"/>
-      <c r="N2559" s="46"/>
-      <c r="V2559" s="46"/>
-    </row>
-    <row r="2560" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2560" s="49"/>
-      <c r="N2560" s="46"/>
-      <c r="V2560" s="46"/>
-    </row>
-    <row r="2561" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2561" s="49"/>
-      <c r="N2561" s="46"/>
-      <c r="V2561" s="46"/>
-    </row>
-    <row r="2562" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2562" s="49"/>
-      <c r="N2562" s="46"/>
-      <c r="V2562" s="46"/>
-    </row>
-    <row r="2563" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2563" s="49"/>
-      <c r="N2563" s="46"/>
-      <c r="V2563" s="46"/>
-    </row>
-    <row r="2564" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2564" s="49"/>
-      <c r="N2564" s="46"/>
-      <c r="V2564" s="46"/>
-    </row>
-    <row r="2565" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2565" s="49"/>
-      <c r="N2565" s="46"/>
-      <c r="V2565" s="46"/>
-    </row>
-    <row r="2566" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2566" s="49"/>
-      <c r="N2566" s="46"/>
-      <c r="V2566" s="46"/>
-    </row>
-    <row r="2567" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2567" s="49"/>
-      <c r="N2567" s="46"/>
-      <c r="V2567" s="46"/>
-    </row>
-    <row r="2568" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2568" s="49"/>
-      <c r="N2568" s="46"/>
-      <c r="V2568" s="46"/>
-    </row>
-    <row r="2569" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2569" s="49"/>
-      <c r="N2569" s="46"/>
-      <c r="V2569" s="46"/>
-    </row>
-    <row r="2570" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2570" s="49"/>
-      <c r="N2570" s="46"/>
-      <c r="V2570" s="46"/>
-    </row>
-    <row r="2571" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2571" s="49"/>
-      <c r="N2571" s="46"/>
-      <c r="V2571" s="46"/>
-    </row>
-    <row r="2572" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2572" s="49"/>
-      <c r="N2572" s="46"/>
-      <c r="V2572" s="46"/>
-    </row>
-    <row r="2573" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2573" s="49"/>
-      <c r="N2573" s="46"/>
-      <c r="V2573" s="46"/>
-    </row>
-    <row r="2574" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2574" s="49"/>
-      <c r="N2574" s="46"/>
-      <c r="V2574" s="46"/>
-    </row>
-    <row r="2575" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2575" s="49"/>
-      <c r="N2575" s="46"/>
-      <c r="V2575" s="46"/>
-    </row>
-    <row r="2576" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2576" s="49"/>
-      <c r="N2576" s="46"/>
-      <c r="V2576" s="46"/>
-    </row>
-    <row r="2577" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2577" s="49"/>
-      <c r="N2577" s="46"/>
-      <c r="V2577" s="46"/>
-    </row>
-    <row r="2578" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2578" s="49"/>
-      <c r="N2578" s="46"/>
-      <c r="V2578" s="46"/>
-    </row>
-    <row r="2579" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2579" s="49"/>
-      <c r="N2579" s="46"/>
-      <c r="V2579" s="46"/>
-    </row>
-    <row r="2580" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2580" s="49"/>
-      <c r="N2580" s="46"/>
-      <c r="V2580" s="46"/>
-    </row>
-    <row r="2581" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2581" s="49"/>
-      <c r="N2581" s="46"/>
-      <c r="V2581" s="46"/>
-    </row>
-    <row r="2582" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2582" s="49"/>
-      <c r="N2582" s="46"/>
-      <c r="V2582" s="46"/>
-    </row>
-    <row r="2583" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2583" s="49"/>
-      <c r="N2583" s="46"/>
-      <c r="V2583" s="46"/>
-    </row>
-    <row r="2584" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2584" s="49"/>
-      <c r="N2584" s="46"/>
-      <c r="V2584" s="46"/>
-    </row>
-    <row r="2585" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2585" s="49"/>
-      <c r="N2585" s="46"/>
-      <c r="V2585" s="46"/>
-    </row>
-    <row r="2586" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2586" s="49"/>
-      <c r="N2586" s="46"/>
-      <c r="V2586" s="46"/>
-    </row>
-    <row r="2587" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2587" s="49"/>
-      <c r="N2587" s="46"/>
-      <c r="V2587" s="46"/>
-    </row>
-    <row r="2588" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2588" s="49"/>
-      <c r="N2588" s="46"/>
-      <c r="V2588" s="46"/>
-    </row>
-    <row r="2589" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2589" s="49"/>
-      <c r="N2589" s="46"/>
-      <c r="V2589" s="46"/>
-    </row>
-    <row r="2590" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2590" s="49"/>
-      <c r="N2590" s="46"/>
-      <c r="V2590" s="46"/>
-    </row>
-    <row r="2591" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2591" s="49"/>
-      <c r="N2591" s="46"/>
-      <c r="V2591" s="46"/>
-    </row>
-    <row r="2592" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2592" s="49"/>
-      <c r="N2592" s="46"/>
-      <c r="V2592" s="46"/>
-    </row>
-    <row r="2593" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2593" s="49"/>
-      <c r="N2593" s="46"/>
-      <c r="V2593" s="46"/>
-    </row>
-    <row r="2594" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2594" s="49"/>
-      <c r="N2594" s="46"/>
-      <c r="V2594" s="46"/>
-    </row>
-    <row r="2595" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2595" s="49"/>
-      <c r="N2595" s="46"/>
-      <c r="V2595" s="46"/>
-    </row>
-    <row r="2596" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2596" s="49"/>
-      <c r="N2596" s="46"/>
-      <c r="V2596" s="46"/>
-    </row>
-    <row r="2597" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2597" s="49"/>
-      <c r="N2597" s="46"/>
-      <c r="V2597" s="46"/>
-    </row>
-    <row r="2598" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2598" s="49"/>
-      <c r="N2598" s="46"/>
-      <c r="V2598" s="46"/>
-    </row>
-    <row r="2599" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2599" s="49"/>
-      <c r="N2599" s="46"/>
-      <c r="V2599" s="46"/>
-    </row>
-    <row r="2600" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2600" s="49"/>
-      <c r="N2600" s="46"/>
-      <c r="V2600" s="46"/>
-    </row>
-    <row r="2601" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2601" s="49"/>
-      <c r="N2601" s="46"/>
-      <c r="V2601" s="46"/>
-    </row>
-    <row r="2602" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2602" s="49"/>
-      <c r="N2602" s="46"/>
-      <c r="V2602" s="46"/>
-    </row>
-    <row r="2603" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2603" s="49"/>
-      <c r="N2603" s="46"/>
-      <c r="V2603" s="46"/>
-    </row>
-    <row r="2604" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2604" s="49"/>
-      <c r="N2604" s="46"/>
-      <c r="V2604" s="46"/>
-    </row>
-    <row r="2605" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2605" s="49"/>
-      <c r="N2605" s="46"/>
-      <c r="V2605" s="46"/>
-    </row>
-    <row r="2606" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2606" s="49"/>
-      <c r="N2606" s="46"/>
-      <c r="V2606" s="46"/>
-    </row>
-    <row r="2607" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2607" s="49"/>
-      <c r="N2607" s="46"/>
-      <c r="V2607" s="46"/>
-    </row>
-    <row r="2608" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2608" s="49"/>
-      <c r="N2608" s="46"/>
-      <c r="V2608" s="46"/>
-    </row>
-    <row r="2609" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2609" s="49"/>
-      <c r="N2609" s="46"/>
-      <c r="V2609" s="46"/>
-    </row>
-    <row r="2610" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2610" s="49"/>
-      <c r="N2610" s="46"/>
-      <c r="V2610" s="46"/>
-    </row>
-    <row r="2611" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2611" s="49"/>
-      <c r="N2611" s="46"/>
-      <c r="V2611" s="46"/>
-    </row>
-    <row r="2612" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2612" s="49"/>
-      <c r="N2612" s="46"/>
-      <c r="V2612" s="46"/>
-    </row>
-    <row r="2613" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2613" s="49"/>
-      <c r="N2613" s="46"/>
-      <c r="V2613" s="46"/>
-    </row>
-    <row r="2614" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2614" s="49"/>
-      <c r="N2614" s="46"/>
-      <c r="V2614" s="46"/>
-    </row>
-    <row r="2615" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2615" s="49"/>
-      <c r="N2615" s="46"/>
-      <c r="V2615" s="46"/>
-    </row>
-    <row r="2616" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2616" s="49"/>
-      <c r="N2616" s="46"/>
-      <c r="V2616" s="46"/>
-    </row>
-    <row r="2617" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2617" s="49"/>
-      <c r="N2617" s="46"/>
-      <c r="V2617" s="46"/>
-    </row>
-    <row r="2618" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2618" s="49"/>
-      <c r="N2618" s="46"/>
-      <c r="V2618" s="46"/>
-    </row>
-    <row r="2619" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2619" s="49"/>
-      <c r="N2619" s="46"/>
-      <c r="V2619" s="46"/>
-    </row>
-    <row r="2620" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2620" s="49"/>
-      <c r="N2620" s="46"/>
-      <c r="V2620" s="46"/>
-    </row>
-    <row r="2621" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2621" s="49"/>
-      <c r="N2621" s="46"/>
-      <c r="V2621" s="46"/>
-    </row>
-    <row r="2622" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2622" s="49"/>
-      <c r="N2622" s="46"/>
-      <c r="V2622" s="46"/>
-    </row>
-    <row r="2623" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2623" s="49"/>
-      <c r="N2623" s="46"/>
-      <c r="V2623" s="46"/>
-    </row>
-    <row r="2624" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2624" s="49"/>
-      <c r="N2624" s="46"/>
-      <c r="V2624" s="46"/>
-    </row>
-    <row r="2625" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2625" s="49"/>
-      <c r="N2625" s="46"/>
-      <c r="V2625" s="46"/>
-    </row>
-    <row r="2626" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2626" s="49"/>
-      <c r="N2626" s="46"/>
-      <c r="V2626" s="46"/>
-    </row>
-    <row r="2627" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2627" s="49"/>
-      <c r="N2627" s="46"/>
-      <c r="V2627" s="46"/>
-    </row>
-    <row r="2628" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2628" s="49"/>
-      <c r="N2628" s="46"/>
-      <c r="V2628" s="46"/>
-    </row>
-    <row r="2629" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2629" s="49"/>
-      <c r="N2629" s="46"/>
-      <c r="V2629" s="46"/>
-    </row>
-    <row r="2630" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2630" s="49"/>
-      <c r="N2630" s="46"/>
-      <c r="V2630" s="46"/>
-    </row>
-    <row r="2631" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2631" s="49"/>
-      <c r="N2631" s="46"/>
-      <c r="V2631" s="46"/>
-    </row>
-    <row r="2632" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2632" s="49"/>
-      <c r="N2632" s="46"/>
-      <c r="V2632" s="46"/>
-    </row>
-    <row r="2633" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2633" s="49"/>
-      <c r="N2633" s="46"/>
-      <c r="V2633" s="46"/>
-    </row>
-    <row r="2634" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2634" s="49"/>
-      <c r="N2634" s="46"/>
-      <c r="V2634" s="46"/>
-    </row>
-    <row r="2635" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2635" s="49"/>
-      <c r="N2635" s="46"/>
-      <c r="V2635" s="46"/>
-    </row>
-    <row r="2636" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2636" s="49"/>
-      <c r="N2636" s="46"/>
-      <c r="V2636" s="46"/>
-    </row>
-    <row r="2637" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2637" s="49"/>
-      <c r="N2637" s="46"/>
-      <c r="V2637" s="46"/>
-    </row>
-    <row r="2638" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2638" s="49"/>
-      <c r="N2638" s="46"/>
-      <c r="V2638" s="46"/>
-    </row>
-    <row r="2639" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2639" s="49"/>
-      <c r="N2639" s="46"/>
-      <c r="V2639" s="46"/>
-    </row>
-    <row r="2640" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2640" s="49"/>
-      <c r="N2640" s="46"/>
-      <c r="V2640" s="46"/>
-    </row>
-    <row r="2641" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2641" s="49"/>
-      <c r="N2641" s="46"/>
-      <c r="V2641" s="46"/>
-    </row>
-    <row r="2642" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2642" s="49"/>
-      <c r="N2642" s="46"/>
-      <c r="V2642" s="46"/>
-    </row>
-    <row r="2643" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2643" s="49"/>
-      <c r="N2643" s="46"/>
-      <c r="V2643" s="46"/>
-    </row>
-    <row r="2644" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2644" s="49"/>
-      <c r="N2644" s="46"/>
-      <c r="V2644" s="46"/>
-    </row>
-    <row r="2645" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2645" s="49"/>
-      <c r="N2645" s="46"/>
-      <c r="V2645" s="46"/>
-    </row>
-    <row r="2646" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2646" s="49"/>
-      <c r="N2646" s="46"/>
-      <c r="V2646" s="46"/>
-    </row>
-    <row r="2647" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2647" s="49"/>
-      <c r="N2647" s="46"/>
-      <c r="V2647" s="46"/>
-    </row>
-    <row r="2648" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2648" s="49"/>
-      <c r="N2648" s="46"/>
-      <c r="V2648" s="46"/>
-    </row>
-    <row r="2649" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2649" s="49"/>
-      <c r="N2649" s="46"/>
-      <c r="V2649" s="46"/>
-    </row>
-    <row r="2650" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2650" s="49"/>
-      <c r="N2650" s="46"/>
-      <c r="V2650" s="46"/>
-    </row>
-    <row r="2651" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2651" s="49"/>
-      <c r="N2651" s="46"/>
-      <c r="V2651" s="46"/>
-    </row>
-    <row r="2652" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2652" s="49"/>
-      <c r="N2652" s="46"/>
-      <c r="V2652" s="46"/>
-    </row>
-    <row r="2653" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2653" s="49"/>
-      <c r="N2653" s="46"/>
-      <c r="V2653" s="46"/>
-    </row>
-    <row r="2654" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2654" s="49"/>
-      <c r="N2654" s="46"/>
-      <c r="V2654" s="46"/>
-    </row>
-    <row r="2655" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2655" s="49"/>
-      <c r="N2655" s="46"/>
-      <c r="V2655" s="46"/>
-    </row>
-    <row r="2656" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2656" s="49"/>
-      <c r="N2656" s="46"/>
-      <c r="V2656" s="46"/>
-    </row>
-    <row r="2657" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2657" s="49"/>
-      <c r="N2657" s="46"/>
-      <c r="V2657" s="46"/>
-    </row>
-    <row r="2658" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2658" s="49"/>
-      <c r="N2658" s="46"/>
-      <c r="V2658" s="46"/>
-    </row>
-    <row r="2659" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2659" s="49"/>
-      <c r="N2659" s="46"/>
-      <c r="V2659" s="46"/>
-    </row>
-    <row r="2660" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2660" s="49"/>
-      <c r="N2660" s="46"/>
-      <c r="V2660" s="46"/>
-    </row>
-    <row r="2661" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2661" s="49"/>
-      <c r="N2661" s="46"/>
-      <c r="V2661" s="46"/>
-    </row>
-    <row r="2662" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2662" s="49"/>
-      <c r="N2662" s="46"/>
-      <c r="V2662" s="46"/>
-    </row>
-    <row r="2663" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2663" s="49"/>
-      <c r="N2663" s="46"/>
-      <c r="V2663" s="46"/>
-    </row>
-    <row r="2664" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2664" s="49"/>
-      <c r="N2664" s="46"/>
-      <c r="V2664" s="46"/>
-    </row>
-    <row r="2665" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2665" s="49"/>
-      <c r="N2665" s="46"/>
-      <c r="V2665" s="46"/>
-    </row>
-    <row r="2666" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2666" s="49"/>
-      <c r="N2666" s="46"/>
-      <c r="V2666" s="46"/>
-    </row>
-    <row r="2667" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2667" s="49"/>
-      <c r="N2667" s="46"/>
-      <c r="V2667" s="46"/>
-    </row>
-    <row r="2668" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2668" s="49"/>
-      <c r="N2668" s="46"/>
-      <c r="V2668" s="46"/>
-    </row>
-    <row r="2669" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2669" s="49"/>
-      <c r="N2669" s="46"/>
-      <c r="V2669" s="46"/>
-    </row>
-    <row r="2670" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2670" s="49"/>
-      <c r="N2670" s="46"/>
-      <c r="V2670" s="46"/>
-    </row>
-    <row r="2671" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2671" s="49"/>
-      <c r="N2671" s="46"/>
-      <c r="V2671" s="46"/>
-    </row>
-    <row r="2672" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2672" s="49"/>
-      <c r="N2672" s="46"/>
-      <c r="V2672" s="46"/>
-    </row>
-    <row r="2673" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2673" s="49"/>
-      <c r="N2673" s="46"/>
-      <c r="V2673" s="46"/>
-    </row>
-    <row r="2674" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2674" s="49"/>
-      <c r="N2674" s="46"/>
-      <c r="V2674" s="46"/>
-    </row>
-    <row r="2675" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2675" s="49"/>
-      <c r="N2675" s="46"/>
-      <c r="V2675" s="46"/>
-    </row>
-    <row r="2676" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2676" s="49"/>
-      <c r="N2676" s="46"/>
-      <c r="V2676" s="46"/>
-    </row>
-    <row r="2677" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2677" s="49"/>
-      <c r="N2677" s="46"/>
-      <c r="V2677" s="46"/>
-    </row>
-    <row r="2678" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2678" s="49"/>
-      <c r="N2678" s="46"/>
-      <c r="V2678" s="46"/>
-    </row>
-    <row r="2679" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2679" s="49"/>
-      <c r="N2679" s="46"/>
-      <c r="V2679" s="46"/>
-    </row>
-    <row r="2680" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2680" s="49"/>
-      <c r="N2680" s="46"/>
-      <c r="V2680" s="46"/>
-    </row>
-    <row r="2681" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2681" s="49"/>
-      <c r="N2681" s="46"/>
-      <c r="V2681" s="46"/>
-    </row>
-    <row r="2682" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2682" s="49"/>
-      <c r="N2682" s="46"/>
-      <c r="V2682" s="46"/>
-    </row>
-    <row r="2683" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2683" s="49"/>
-      <c r="N2683" s="46"/>
-      <c r="V2683" s="46"/>
-    </row>
-    <row r="2684" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2684" s="49"/>
-      <c r="N2684" s="46"/>
-      <c r="V2684" s="46"/>
-    </row>
-    <row r="2685" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2685" s="49"/>
-      <c r="N2685" s="46"/>
-      <c r="V2685" s="46"/>
-    </row>
-    <row r="2686" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2686" s="49"/>
-      <c r="N2686" s="46"/>
-      <c r="V2686" s="46"/>
-    </row>
-    <row r="2687" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2687" s="49"/>
-      <c r="N2687" s="46"/>
-      <c r="V2687" s="46"/>
-    </row>
-    <row r="2688" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2688" s="49"/>
-      <c r="N2688" s="46"/>
-      <c r="V2688" s="46"/>
-    </row>
-    <row r="2689" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2689" s="49"/>
-      <c r="N2689" s="46"/>
-      <c r="V2689" s="46"/>
-    </row>
-    <row r="2690" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2690" s="49"/>
-      <c r="N2690" s="46"/>
-      <c r="V2690" s="46"/>
-    </row>
-    <row r="2691" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2691" s="49"/>
-      <c r="N2691" s="46"/>
-      <c r="V2691" s="46"/>
-    </row>
-    <row r="2692" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2692" s="49"/>
-      <c r="N2692" s="46"/>
-      <c r="V2692" s="46"/>
-    </row>
-    <row r="2693" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2693" s="49"/>
-      <c r="N2693" s="46"/>
-      <c r="V2693" s="46"/>
-    </row>
-    <row r="2694" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2694" s="49"/>
-      <c r="N2694" s="46"/>
-      <c r="V2694" s="46"/>
-    </row>
-    <row r="2695" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2695" s="49"/>
-      <c r="N2695" s="46"/>
-      <c r="V2695" s="46"/>
-    </row>
-    <row r="2696" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2696" s="49"/>
-      <c r="N2696" s="46"/>
-      <c r="V2696" s="46"/>
-    </row>
-    <row r="2697" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2697" s="49"/>
-      <c r="N2697" s="46"/>
-      <c r="V2697" s="46"/>
-    </row>
-    <row r="2698" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2698" s="49"/>
-      <c r="N2698" s="46"/>
-      <c r="V2698" s="46"/>
-    </row>
-    <row r="2699" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2699" s="49"/>
-      <c r="N2699" s="46"/>
-      <c r="V2699" s="46"/>
-    </row>
-    <row r="2700" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2700" s="49"/>
-      <c r="N2700" s="46"/>
-      <c r="V2700" s="46"/>
-    </row>
-    <row r="2701" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2701" s="49"/>
-      <c r="N2701" s="46"/>
-      <c r="V2701" s="46"/>
-    </row>
-    <row r="2702" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2702" s="49"/>
-      <c r="N2702" s="46"/>
-      <c r="V2702" s="46"/>
-    </row>
-    <row r="2703" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2703" s="49"/>
-      <c r="N2703" s="46"/>
-      <c r="V2703" s="46"/>
-    </row>
-    <row r="2704" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2704" s="49"/>
-      <c r="N2704" s="46"/>
-      <c r="V2704" s="46"/>
-    </row>
-    <row r="2705" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2705" s="49"/>
-      <c r="N2705" s="46"/>
-      <c r="V2705" s="46"/>
-    </row>
-    <row r="2706" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2706" s="49"/>
-      <c r="N2706" s="46"/>
-      <c r="V2706" s="46"/>
-    </row>
-    <row r="2707" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2707" s="49"/>
-      <c r="N2707" s="46"/>
-      <c r="V2707" s="46"/>
-    </row>
-    <row r="2708" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2708" s="49"/>
-      <c r="N2708" s="46"/>
-      <c r="V2708" s="46"/>
-    </row>
-    <row r="2709" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2709" s="49"/>
-      <c r="N2709" s="46"/>
-      <c r="V2709" s="46"/>
-    </row>
-    <row r="2710" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2710" s="49"/>
-      <c r="N2710" s="46"/>
-      <c r="V2710" s="46"/>
-    </row>
-    <row r="2711" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2711" s="49"/>
-      <c r="N2711" s="46"/>
-      <c r="V2711" s="46"/>
-    </row>
-    <row r="2712" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2712" s="49"/>
-      <c r="N2712" s="46"/>
-      <c r="V2712" s="46"/>
-    </row>
-    <row r="2713" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2713" s="49"/>
-      <c r="N2713" s="46"/>
-      <c r="V2713" s="46"/>
-    </row>
-    <row r="2714" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2714" s="49"/>
-      <c r="N2714" s="46"/>
-      <c r="V2714" s="46"/>
-    </row>
-    <row r="2715" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2715" s="49"/>
-      <c r="N2715" s="46"/>
-      <c r="V2715" s="46"/>
-    </row>
-    <row r="2716" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2716" s="49"/>
-      <c r="N2716" s="46"/>
-      <c r="V2716" s="46"/>
-    </row>
-    <row r="2717" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2717" s="49"/>
-      <c r="N2717" s="46"/>
-      <c r="V2717" s="46"/>
-    </row>
-    <row r="2718" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2718" s="49"/>
-      <c r="N2718" s="46"/>
-      <c r="V2718" s="46"/>
-    </row>
-    <row r="2719" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2719" s="49"/>
-      <c r="N2719" s="46"/>
-      <c r="V2719" s="46"/>
-    </row>
-    <row r="2720" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2720" s="49"/>
-      <c r="N2720" s="46"/>
-      <c r="V2720" s="46"/>
-    </row>
-    <row r="2721" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2721" s="49"/>
-      <c r="N2721" s="46"/>
-      <c r="V2721" s="46"/>
-    </row>
-    <row r="2722" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2722" s="49"/>
-      <c r="N2722" s="46"/>
-      <c r="V2722" s="46"/>
-    </row>
-    <row r="2723" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2723" s="49"/>
-      <c r="N2723" s="46"/>
-      <c r="V2723" s="46"/>
-    </row>
-    <row r="2724" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2724" s="49"/>
-      <c r="N2724" s="46"/>
-      <c r="V2724" s="46"/>
-    </row>
-    <row r="2725" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2725" s="49"/>
-      <c r="N2725" s="46"/>
-      <c r="V2725" s="46"/>
-    </row>
-    <row r="2726" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2726" s="49"/>
-      <c r="N2726" s="46"/>
-      <c r="V2726" s="46"/>
-    </row>
-    <row r="2727" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2727" s="49"/>
-      <c r="N2727" s="46"/>
-      <c r="V2727" s="46"/>
-    </row>
-    <row r="2728" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I2728" s="49"/>
-      <c r="N2728" s="46"/>
-      <c r="V2728" s="46"/>
     </row>
   </sheetData>
   <autoFilter ref="C1:V2331" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
nmv 19 12 2023
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 7.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 7.2 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB872E44-0985-47C7-AFE1-037EFC459106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295AAE22-0127-4BC9-A5A1-B5FEC6046ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6071" uniqueCount="1181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6071" uniqueCount="1180">
   <si>
     <t>Passage</t>
   </si>
@@ -3538,9 +3538,6 @@
   </si>
   <si>
     <t>P[r]</t>
-  </si>
-  <si>
-    <t>P[r]+S{r]</t>
   </si>
   <si>
     <t>P[r]+S[r]+N[r]</t>
@@ -3791,7 +3788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3979,21 +3976,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4286,7 +4268,7 @@
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="S2331" sqref="S2331"/>
+      <selection pane="bottomLeft" activeCell="N1481" sqref="N1481"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -10289,7 +10271,7 @@
         <f t="shared" si="8"/>
         <v>146</v>
       </c>
-      <c r="N147" s="70" t="s">
+      <c r="N147" s="65" t="s">
         <v>212</v>
       </c>
       <c r="O147" s="7"/>
@@ -10303,7 +10285,7 @@
     </row>
     <row r="148" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A148" s="57" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B148" s="57"/>
       <c r="C148" s="57"/>
@@ -10329,7 +10311,7 @@
         <f t="shared" si="8"/>
         <v>147</v>
       </c>
-      <c r="N148" s="70" t="s">
+      <c r="N148" s="65" t="s">
         <v>213</v>
       </c>
       <c r="O148" s="7"/>
@@ -16580,7 +16562,7 @@
         <v>116</v>
       </c>
       <c r="N328" s="46" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="O328" s="8" t="s">
         <v>73</v>
@@ -22487,7 +22469,7 @@
       <c r="S499" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="T499" s="69" t="s">
+      <c r="T499" s="64" t="s">
         <v>78</v>
       </c>
       <c r="U499" s="8"/>
@@ -22527,8 +22509,8 @@
       <c r="S500" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="T500" s="69" t="s">
-        <v>1180</v>
+      <c r="T500" s="64" t="s">
+        <v>1179</v>
       </c>
       <c r="U500" s="8"/>
       <c r="V500" s="46"/>
@@ -27616,7 +27598,7 @@
         <v>61</v>
       </c>
       <c r="N648" s="47" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="O648" s="8" t="s">
         <v>70</v>
@@ -44517,35 +44499,35 @@
     </row>
     <row r="1167" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="H1167" s="31"/>
-      <c r="I1167" s="64" t="s">
+      <c r="I1167" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="J1167" s="65">
+      <c r="J1167" s="52">
         <v>24</v>
       </c>
-      <c r="K1167" s="66">
+      <c r="K1167" s="6">
         <f t="shared" si="54"/>
         <v>1166</v>
       </c>
-      <c r="L1167" s="66">
+      <c r="L1167" s="6">
         <f t="shared" si="55"/>
         <v>50</v>
       </c>
-      <c r="M1167" s="66">
+      <c r="M1167" s="6">
         <f t="shared" si="56"/>
         <v>150</v>
       </c>
-      <c r="N1167" s="67" t="s">
+      <c r="N1167" s="46" t="s">
         <v>590</v>
       </c>
-      <c r="O1167" s="68"/>
-      <c r="P1167" s="68"/>
-      <c r="Q1167" s="68"/>
-      <c r="R1167" s="68"/>
-      <c r="S1167" s="68"/>
-      <c r="T1167" s="68"/>
-      <c r="U1167" s="68"/>
-      <c r="V1167" s="67"/>
+      <c r="O1167" s="8"/>
+      <c r="P1167" s="8"/>
+      <c r="Q1167" s="8"/>
+      <c r="R1167" s="8"/>
+      <c r="S1167" s="8"/>
+      <c r="T1167" s="8"/>
+      <c r="U1167" s="8"/>
+      <c r="V1167" s="46"/>
     </row>
     <row r="1168" spans="4:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1168" s="49" t="s">
@@ -51422,7 +51404,7 @@
     </row>
     <row r="1381" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1381" s="62" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="C1381" s="41"/>
       <c r="H1381" s="34"/>
@@ -51458,7 +51440,7 @@
     </row>
     <row r="1382" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1382" s="8" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C1382" s="41"/>
       <c r="H1382" s="34"/>
@@ -51496,7 +51478,7 @@
     </row>
     <row r="1383" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1383" s="8" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C1383" s="41"/>
       <c r="H1383" s="34"/>
@@ -53898,7 +53880,7 @@
     </row>
     <row r="1456" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1456" s="62" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C1456" s="41"/>
       <c r="I1456" s="49" t="s">
@@ -53933,7 +53915,7 @@
     </row>
     <row r="1457" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1457" s="8" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C1457" s="41"/>
       <c r="I1457" s="49" t="s">
@@ -53968,7 +53950,7 @@
     </row>
     <row r="1458" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1458" s="8" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C1458" s="41"/>
       <c r="G1458" s="34"/>
@@ -54777,8 +54759,8 @@
       <c r="S1481" s="8" t="s">
         <v>1166</v>
       </c>
-      <c r="T1481" s="8" t="s">
-        <v>1170</v>
+      <c r="T1481" s="64" t="s">
+        <v>1167</v>
       </c>
       <c r="U1481" s="8"/>
       <c r="V1481" s="46"/>
@@ -55932,7 +55914,7 @@
     </row>
     <row r="1517" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1517" s="62" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="C1517" s="41"/>
       <c r="I1517" s="49" t="s">
@@ -55967,7 +55949,7 @@
     </row>
     <row r="1518" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1518" s="8" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C1518" s="41"/>
       <c r="I1518" s="49" t="s">
@@ -55999,12 +55981,12 @@
       <c r="R1518" s="8"/>
       <c r="S1518" s="8"/>
       <c r="T1518" s="8"/>
-      <c r="U1518" s="69"/>
+      <c r="U1518" s="64"/>
       <c r="V1518" s="46"/>
     </row>
     <row r="1519" spans="1:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1519" s="8" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C1519" s="41"/>
       <c r="I1519" s="49" t="s">
@@ -56646,7 +56628,7 @@
         <v>1166</v>
       </c>
       <c r="T1537" s="8" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="U1537" s="8"/>
       <c r="V1537" s="46"/>
@@ -66778,10 +66760,10 @@
         <v>809</v>
       </c>
       <c r="S1922" s="1" t="s">
+        <v>1173</v>
+      </c>
+      <c r="T1922" s="1" t="s">
         <v>1174</v>
-      </c>
-      <c r="T1922" s="1" t="s">
-        <v>1175</v>
       </c>
       <c r="V1922" s="46"/>
     </row>

</xml_diff>

<commit_message>
nmv 27 03 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Templates/TS 7.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Templates/TS 7.2 Padam Input Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Working\Padam Input Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57513095-FCE7-42B5-9291-1154920ABF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03061DD9-7769-4734-A30C-0A12FF50F3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6069" uniqueCount="1177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6068" uniqueCount="1177">
   <si>
     <t>Passage</t>
   </si>
@@ -3549,9 +3549,6 @@
     <t>anu cChandaH</t>
   </si>
   <si>
-    <t>prA~g. yAnti (swara bakthi??)</t>
-  </si>
-  <si>
     <t>jyoti#HpakShA</t>
   </si>
   <si>
@@ -3559,6 +3556,9 @@
   </si>
   <si>
     <t>ASva#tthIq ityASva#tthI</t>
+  </si>
+  <si>
+    <t>var.Sha$t</t>
   </si>
 </sst>
 </file>
@@ -4256,10 +4256,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2318" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N657" sqref="N657"/>
+      <selection pane="bottomLeft" activeCell="N1381" sqref="N1381:N1382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6489,7 +6489,7 @@
         <v>43</v>
       </c>
       <c r="N44" s="47" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="O44" s="8" t="s">
         <v>70</v>
@@ -9603,7 +9603,7 @@
       <c r="T128" s="8"/>
       <c r="U128" s="8"/>
       <c r="V128" s="47" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="129" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10275,9 +10275,7 @@
       <c r="V147" s="46"/>
     </row>
     <row r="148" spans="1:22" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A148" s="57" t="s">
-        <v>1173</v>
-      </c>
+      <c r="A148" s="57"/>
       <c r="B148" s="57"/>
       <c r="C148" s="57"/>
       <c r="D148" s="24"/>
@@ -47833,7 +47831,7 @@
         <v>255</v>
       </c>
       <c r="N1272" s="47" t="s">
-        <v>626</v>
+        <v>1176</v>
       </c>
       <c r="O1272" s="7"/>
       <c r="P1272" s="8"/>
@@ -61999,7 +61997,7 @@
         <v>93</v>
       </c>
       <c r="N1736" s="47" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="O1736" s="8" t="s">
         <v>70</v>

</xml_diff>